<commit_message>
updates para pasarlo a un pdf
</commit_message>
<xml_diff>
--- a/HT-1/Banco-BAC-10-Catálogo de conceptos.xlsx
+++ b/HT-1/Banco-BAC-10-Catálogo de conceptos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juan/Documents/Universidad/2022-20/arquiemp/repo/arquiemp/HT-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ADD5943-DD6D-794A-B145-62DAF4F36BCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D60BE0-CAFD-C949-9245-F9B1A578FFFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{6D2ADF59-F33A-44E3-88FB-8431094B32CC}"/>
   </bookViews>
@@ -93,9 +93,6 @@
     <t>Préstamo</t>
   </si>
   <si>
-    <t>Sede</t>
-  </si>
-  <si>
     <t>Colchón</t>
   </si>
   <si>
@@ -136,6 +133,9 @@
   </si>
   <si>
     <t>Individuo, ser humano</t>
+  </si>
+  <si>
+    <t>Sede, oficina</t>
   </si>
 </sst>
 </file>
@@ -538,7 +538,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -591,7 +591,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>17</v>
@@ -602,7 +602,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>18</v>
@@ -613,10 +613,10 @@
         <v>10</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.15">
@@ -624,10 +624,10 @@
         <v>3</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.15">
@@ -635,10 +635,10 @@
         <v>11</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.15">
@@ -646,10 +646,10 @@
         <v>12</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.15">
@@ -657,7 +657,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C13" s="6"/>
     </row>
@@ -666,10 +666,10 @@
         <v>14</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.15">
@@ -677,10 +677,10 @@
         <v>15</v>
       </c>
       <c r="B15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>32</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>